<commit_message>
add load_cvs in nand configuration
</commit_message>
<xml_diff>
--- a/config/nand_128gb_mlc.xlsx
+++ b/config/nand_128gb_mlc.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{2EEA005B-9DD8-D948-A7CA-EE815B6FE851}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{B2E85CEF-8EDE-9347-BFFD-EACD2FB3BAFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>bits_per_cell</t>
   </si>

</xml_diff>